<commit_message>
Initial commit for States game and final commit for AD
</commit_message>
<xml_diff>
--- a/TLRS/dist/server2022.xlsx
+++ b/TLRS/dist/server2022.xlsx
@@ -14,15 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>HSKD22WS001@retail.spar.co.za</t>
-  </si>
-  <si>
-    <t>HSKD22WS002@retail.spar.co.za</t>
-  </si>
-  <si>
-    <t>HSKD22SRV001@retail.spar.co.za</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>HENNOWS001@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS002@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS003@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS004@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS005@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS006@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS007@retail.spar.co.za</t>
+  </si>
+  <si>
+    <t>HENNOWS008@retail.spar.co.za</t>
   </si>
 </sst>
 </file>
@@ -354,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -375,6 +390,31 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>